<commit_message>
Clean up after test
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rosericazondekon/Documents/CiBIGR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C1C6456-477C-FD4B-AEE8-A03A829B48F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E199BD3-C80C-9E40-A196-74FC032FCAFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="800" windowWidth="15800" windowHeight="13060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="800" windowWidth="17140" windowHeight="13600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -374,7 +374,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>